<commit_message>
updated excel for import
</commit_message>
<xml_diff>
--- a/import_this_excel_example.xlsx
+++ b/import_this_excel_example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -440,7 +440,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -450,13 +450,15 @@
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -628,12 +630,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="L2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="L3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="L4" r:id="rId6"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="L4" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>